<commit_message>
created new test for products page
</commit_message>
<xml_diff>
--- a/FinalProject-AutomationExercise-Data.xlsx
+++ b/FinalProject-AutomationExercise-Data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitic\IdeaProjects\FinalProject-AutomationExcercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC2DC4C-0787-48CF-81A4-CE3846090291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13031F8E-6C09-4561-B0BF-F2E54BD36C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="1815" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23040" yWindow="612" windowWidth="21600" windowHeight="11292" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SignUpData" sheetId="1" r:id="rId1"/>
+    <sheet name="SignUpDataValid" sheetId="1" r:id="rId1"/>
+    <sheet name="CreatedUserData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="37">
   <si>
     <t>Title</t>
   </si>
@@ -75,21 +76,12 @@
     <t>Mobile number</t>
   </si>
   <si>
-    <t>Marko</t>
-  </si>
-  <si>
-    <t>marko@qa</t>
-  </si>
-  <si>
     <t>QwertY123!@#</t>
   </si>
   <si>
     <t>QA ltd</t>
   </si>
   <si>
-    <t>Adress 1</t>
-  </si>
-  <si>
     <t>India</t>
   </si>
   <si>
@@ -109,13 +101,49 @@
   </si>
   <si>
     <t>Singapore</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>mr</t>
+  </si>
+  <si>
+    <t>Month of Birth</t>
+  </si>
+  <si>
+    <t>Year of Birth</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>mark@qa</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>794 Mcallister St</t>
+  </si>
+  <si>
+    <t>66 Ceres St</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>San Francisko</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +158,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -153,9 +187,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -437,146 +473,425 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="5" max="7" width="17.28515625" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" customWidth="1"/>
-    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" customWidth="1"/>
+    <col min="18" max="18" width="12" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="T1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="M2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="1">
+        <v>94016</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M3" t="s">
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M4" t="s">
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M5" t="s">
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M8" t="s">
-        <v>27</v>
-      </c>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -585,4 +900,435 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E141D381-D645-4E53-B802-91348239F580}">
+  <dimension ref="A1:T14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" customWidth="1"/>
+    <col min="18" max="18" width="12" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="1">
+        <v>94016</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{53BE86EF-60FB-4302-ACD1-FE6A4D7AE781}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{9BD13DA4-E853-4176-AE77-9D1F4A654BDB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated test for mandatory fields signup
</commit_message>
<xml_diff>
--- a/FinalProject-AutomationExercise-Data.xlsx
+++ b/FinalProject-AutomationExercise-Data.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitic\IdeaProjects\FinalProject-AutomationExcercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13031F8E-6C09-4561-B0BF-F2E54BD36C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF2BE67-26D1-4E44-BEFD-A75C8BC1A2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23040" yWindow="612" windowWidth="21600" windowHeight="11292" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23040" yWindow="612" windowWidth="21600" windowHeight="11292" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUpDataValid" sheetId="1" r:id="rId1"/>
     <sheet name="CreatedUserData" sheetId="2" r:id="rId2"/>
+    <sheet name="InvalidData" sheetId="3" r:id="rId3"/>
+    <sheet name="ExistingUser" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="48">
   <si>
     <t>Title</t>
   </si>
@@ -137,6 +139,39 @@
   </si>
   <si>
     <t>San Francisko</t>
+  </si>
+  <si>
+    <t>markqa</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>john@smit.com</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>QA USA ltd</t>
   </si>
 </sst>
 </file>
@@ -475,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E141D381-D645-4E53-B802-91348239F580}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -1331,4 +1366,853 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04F4467-D9FC-4120-8B29-3728EBBABF73}">
+  <dimension ref="A1:T14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" customWidth="1"/>
+    <col min="18" max="18" width="12" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="1">
+        <v>94016</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="mark@qa" xr:uid="{D3E20320-6DE7-40DC-AB60-43CCB9423BD1}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{3FEA59C2-05F6-4758-8F13-03ED9DD5503C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2775CBED-8D32-4BD5-ABEF-CDC0D928B58D}">
+  <dimension ref="A1:T14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" customWidth="1"/>
+    <col min="18" max="18" width="12" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="1">
+        <v>94016</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{0131BEFD-09C3-4A3B-85C2-1201598000C1}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{F06DCAD7-FA3C-495C-9612-6F38CA15967B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>